<commit_message>
add Quality Appraisal results using MINORS tool
</commit_message>
<xml_diff>
--- a/QA 1/QA results/QA results.xlsx
+++ b/QA 1/QA results/QA results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tired_llama\projects\bahmani-sysrev\QA 1\QA results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7624BB8-1A7B-492F-A8BF-F0676777A8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78179D9-D9D7-4928-8A7C-334E71BE6593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cohort" sheetId="1" r:id="rId1"/>
     <sheet name="Case-control" sheetId="2" r:id="rId2"/>
     <sheet name="Cross-sectional" sheetId="3" r:id="rId3"/>
+    <sheet name="MINORS" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="126">
   <si>
     <t>study ID</t>
   </si>
@@ -383,12 +384,57 @@
   <si>
     <t>Low quality</t>
   </si>
+  <si>
+    <t>(1) A clearly stated aim: The question addressed should be precise and relevant in the light of available literature</t>
+  </si>
+  <si>
+    <t>(2) Inclusion of consecutive patients: All patients potentially fir for inclusion (satisfying the criteria for inclusion) have been included in the study during the study period</t>
+  </si>
+  <si>
+    <t>(3) Prospective collection of data: Data were collected according to a protocol established before the beginning of the study.</t>
+  </si>
+  <si>
+    <t>(4) Endpoints appropriate to the aim of the study: Unambiguous explanation of the criteria used to evaluate the main outcome, which should be in accordance with the question addressed by the study. Also, the endpoints should be assessed on an intention-to-treat basis</t>
+  </si>
+  <si>
+    <t>(5) Unbiased assessment of the study endpoint: Blind evaluation of objective endpoints and double-blind evaluation of subjective endpoints. Otherwise the reasons for not blinding should b stated.</t>
+  </si>
+  <si>
+    <t>(6) Follow-up period appropriate to the aim of the study: The follow-up should be sufficiently long to allow the assessment of the main endpoint and possible adverse events</t>
+  </si>
+  <si>
+    <t>(7) Loss to follow up less than 5%: All patient should be included in the follow up. Otherwise, the proportion lost to follow up should not exceed the proportion experiencing the major endpoint</t>
+  </si>
+  <si>
+    <t>(8) Prospective calculation of study size: Information of the size of detectable difference of interest with a calculation of 95% confidence interval, according to the expected incidence of the outcome event, and information about the level for statistical significance and estimates of power when comparing outcomes.</t>
+  </si>
+  <si>
+    <t>(9) An adequate control group: Having a gold standard diagnostic test or therapeutic intervention recognized as the optimal intervention according to the available published data.</t>
+  </si>
+  <si>
+    <t>(10) Contemporary groups: Control and studied group should be managed during the same time period (no historical controls)</t>
+  </si>
+  <si>
+    <t>(11) Baseline equivalence of groups: The groups should be similar regarding the criteria other than the studied endpoints. Absence of confounding factors that could bias the interpretation of results.</t>
+  </si>
+  <si>
+    <t>(12) Adequate statistical analyses: Whether the statistics were in accordance with the type of study with calculation of confidence intervals or relative risk</t>
+  </si>
+  <si>
+    <t>2 (reported and adequate)</t>
+  </si>
+  <si>
+    <t>1 (reported but inadequate)</t>
+  </si>
+  <si>
+    <t>0 (not reported)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,6 +475,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -549,7 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -836,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1139,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E70BFB-2ED7-443C-A36F-FB7451F96D70}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1339,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CDCE7F-A1DD-4952-A845-E200856AD85F}">
   <dimension ref="B1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1471,7 +1524,7 @@
       </c>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="2:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>87</v>
       </c>
@@ -1499,7 +1552,7 @@
       <c r="J7">
         <v>3</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="K7" s="18" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1531,11 +1584,11 @@
       <c r="J8">
         <v>6</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>91</v>
       </c>
@@ -1563,11 +1616,11 @@
       <c r="J9">
         <v>7</v>
       </c>
-      <c r="K9" s="22" t="s">
+      <c r="K9" s="18" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>94</v>
       </c>
@@ -1595,11 +1648,11 @@
       <c r="J10">
         <v>6</v>
       </c>
-      <c r="K10" s="22" t="s">
+      <c r="K10" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>95</v>
       </c>
@@ -1627,11 +1680,11 @@
       <c r="J11">
         <v>6</v>
       </c>
-      <c r="K11" s="22" t="s">
+      <c r="K11" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>97</v>
       </c>
@@ -1659,11 +1712,11 @@
       <c r="J12">
         <v>7</v>
       </c>
-      <c r="K12" s="22" t="s">
+      <c r="K12" s="18" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>98</v>
       </c>
@@ -1691,11 +1744,11 @@
       <c r="J13">
         <v>6</v>
       </c>
-      <c r="K13" s="22" t="s">
+      <c r="K13" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>99</v>
       </c>
@@ -1723,11 +1776,11 @@
       <c r="J14">
         <v>6</v>
       </c>
-      <c r="K14" s="22" t="s">
+      <c r="K14" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>101</v>
       </c>
@@ -1755,7 +1808,7 @@
       <c r="J15">
         <v>7</v>
       </c>
-      <c r="K15" s="22" t="s">
+      <c r="K15" s="18" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1767,4 +1820,785 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFEEB3B2-9409-45F4-B8CB-D7EA5663FF41}">
+  <dimension ref="A1:N18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="14" width="20.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="6" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" t="s">
+        <v>123</v>
+      </c>
+      <c r="K2" t="s">
+        <v>123</v>
+      </c>
+      <c r="L2" t="s">
+        <v>123</v>
+      </c>
+      <c r="M2" t="s">
+        <v>123</v>
+      </c>
+      <c r="N2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" t="s">
+        <v>124</v>
+      </c>
+      <c r="J3" t="s">
+        <v>124</v>
+      </c>
+      <c r="K3" t="s">
+        <v>124</v>
+      </c>
+      <c r="L3" t="s">
+        <v>124</v>
+      </c>
+      <c r="M3" t="s">
+        <v>124</v>
+      </c>
+      <c r="N3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H5" t="s">
+        <v>124</v>
+      </c>
+      <c r="I5" t="s">
+        <v>125</v>
+      </c>
+      <c r="J5" t="s">
+        <v>125</v>
+      </c>
+      <c r="K5" t="s">
+        <v>123</v>
+      </c>
+      <c r="L5" t="s">
+        <v>123</v>
+      </c>
+      <c r="M5" t="s">
+        <v>123</v>
+      </c>
+      <c r="N5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J6" t="s">
+        <v>125</v>
+      </c>
+      <c r="K6" t="s">
+        <v>124</v>
+      </c>
+      <c r="L6" t="s">
+        <v>123</v>
+      </c>
+      <c r="M6" t="s">
+        <v>124</v>
+      </c>
+      <c r="N6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7" t="s">
+        <v>124</v>
+      </c>
+      <c r="H7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I7" t="s">
+        <v>124</v>
+      </c>
+      <c r="J7" t="s">
+        <v>125</v>
+      </c>
+      <c r="K7" t="s">
+        <v>124</v>
+      </c>
+      <c r="L7" t="s">
+        <v>123</v>
+      </c>
+      <c r="M7" t="s">
+        <v>124</v>
+      </c>
+      <c r="N7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G8" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" t="s">
+        <v>124</v>
+      </c>
+      <c r="I8" t="s">
+        <v>123</v>
+      </c>
+      <c r="J8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H9" t="s">
+        <v>123</v>
+      </c>
+      <c r="I9" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" t="s">
+        <v>123</v>
+      </c>
+      <c r="H10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I10" t="s">
+        <v>124</v>
+      </c>
+      <c r="J10" t="s">
+        <v>125</v>
+      </c>
+      <c r="K10" t="s">
+        <v>125</v>
+      </c>
+      <c r="L10" t="s">
+        <v>123</v>
+      </c>
+      <c r="M10" t="s">
+        <v>124</v>
+      </c>
+      <c r="N10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" t="s">
+        <v>123</v>
+      </c>
+      <c r="F11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G11" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" t="s">
+        <v>124</v>
+      </c>
+      <c r="J11" t="s">
+        <v>125</v>
+      </c>
+      <c r="K11" t="s">
+        <v>125</v>
+      </c>
+      <c r="L11" t="s">
+        <v>123</v>
+      </c>
+      <c r="M11" t="s">
+        <v>124</v>
+      </c>
+      <c r="N11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" t="s">
+        <v>123</v>
+      </c>
+      <c r="F12" t="s">
+        <v>123</v>
+      </c>
+      <c r="G12" t="s">
+        <v>123</v>
+      </c>
+      <c r="H12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I12" t="s">
+        <v>124</v>
+      </c>
+      <c r="J12" t="s">
+        <v>125</v>
+      </c>
+      <c r="K12" t="s">
+        <v>125</v>
+      </c>
+      <c r="L12" t="s">
+        <v>123</v>
+      </c>
+      <c r="M12" t="s">
+        <v>125</v>
+      </c>
+      <c r="N12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F13" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13" t="s">
+        <v>123</v>
+      </c>
+      <c r="H13" t="s">
+        <v>123</v>
+      </c>
+      <c r="I13" t="s">
+        <v>125</v>
+      </c>
+      <c r="J13" t="s">
+        <v>123</v>
+      </c>
+      <c r="K13" t="s">
+        <v>125</v>
+      </c>
+      <c r="L13" t="s">
+        <v>123</v>
+      </c>
+      <c r="M13" t="s">
+        <v>124</v>
+      </c>
+      <c r="N13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" t="s">
+        <v>123</v>
+      </c>
+      <c r="F14" t="s">
+        <v>123</v>
+      </c>
+      <c r="G14" t="s">
+        <v>123</v>
+      </c>
+      <c r="H14" t="s">
+        <v>123</v>
+      </c>
+      <c r="I14" t="s">
+        <v>123</v>
+      </c>
+      <c r="J14" t="s">
+        <v>125</v>
+      </c>
+      <c r="K14" t="s">
+        <v>125</v>
+      </c>
+      <c r="L14" t="s">
+        <v>123</v>
+      </c>
+      <c r="M14" t="s">
+        <v>123</v>
+      </c>
+      <c r="N14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" t="s">
+        <v>124</v>
+      </c>
+      <c r="E15" t="s">
+        <v>123</v>
+      </c>
+      <c r="F15" t="s">
+        <v>123</v>
+      </c>
+      <c r="G15" t="s">
+        <v>123</v>
+      </c>
+      <c r="H15" t="s">
+        <v>123</v>
+      </c>
+      <c r="I15" t="s">
+        <v>125</v>
+      </c>
+      <c r="J15" t="s">
+        <v>125</v>
+      </c>
+      <c r="K15" t="s">
+        <v>125</v>
+      </c>
+      <c r="L15" t="s">
+        <v>123</v>
+      </c>
+      <c r="M15" t="s">
+        <v>125</v>
+      </c>
+      <c r="N15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E16" t="s">
+        <v>125</v>
+      </c>
+      <c r="F16" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" t="s">
+        <v>123</v>
+      </c>
+      <c r="I16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J16" t="s">
+        <v>125</v>
+      </c>
+      <c r="K16" t="s">
+        <v>124</v>
+      </c>
+      <c r="L16" t="s">
+        <v>123</v>
+      </c>
+      <c r="M16" t="s">
+        <v>124</v>
+      </c>
+      <c r="N16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F17" t="s">
+        <v>123</v>
+      </c>
+      <c r="G17" t="s">
+        <v>123</v>
+      </c>
+      <c r="H17" t="s">
+        <v>123</v>
+      </c>
+      <c r="I17" t="s">
+        <v>125</v>
+      </c>
+      <c r="J17" t="s">
+        <v>123</v>
+      </c>
+      <c r="K17" t="s">
+        <v>124</v>
+      </c>
+      <c r="L17" t="s">
+        <v>123</v>
+      </c>
+      <c r="M17" t="s">
+        <v>124</v>
+      </c>
+      <c r="N17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F18" t="s">
+        <v>123</v>
+      </c>
+      <c r="G18" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" t="s">
+        <v>123</v>
+      </c>
+      <c r="I18" t="s">
+        <v>125</v>
+      </c>
+      <c r="J18" t="s">
+        <v>125</v>
+      </c>
+      <c r="K18" t="s">
+        <v>124</v>
+      </c>
+      <c r="L18" t="s">
+        <v>123</v>
+      </c>
+      <c r="M18" t="s">
+        <v>124</v>
+      </c>
+      <c r="N18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8:F18 E5:F7 C5:C51" xr:uid="{19680816-1539-4C4F-A73D-9A67169568AB}">
+      <formula1>$C$2:C$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:N8 E8:E104 D5:D104 G5:G104 F19:F104 H9:N104" xr:uid="{E7188BD1-443F-4B08-A494-3B2986669402}">
+      <formula1>D$2:D$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:E10 C11:C15 E11:E12" xr:uid="{1736488A-CD74-45CF-9749-2CD22C285B99}">
+      <formula1>G$2:G$4</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>